<commit_message>
assign name to <blank name> VM in server 2 and server 3
</commit_message>
<xml_diff>
--- a/data/firstData.xlsx
+++ b/data/firstData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BADF0FA-6D70-B844-BB7D-D5A16223542C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639F2A12-9688-4548-8403-C9DA9C5B4C6E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{1AC0D294-ED21-41DD-B61F-C0F05BB4ACE3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="2" xr2:uid="{1AC0D294-ED21-41DD-B61F-C0F05BB4ACE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
   <si>
     <t>dc1</t>
   </si>
@@ -385,6 +385,15 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>none1</t>
+  </si>
+  <si>
+    <t>none2</t>
+  </si>
+  <si>
+    <t>none3</t>
   </si>
 </sst>
 </file>
@@ -810,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5504485-04A0-4EFE-902B-4833CC7B7514}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1148,13 +1157,14 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1359,7 +1369,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="B13" s="7" t="s">
         <v>59</v>
       </c>
@@ -1391,7 +1403,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="B15" s="7" t="s">
         <v>61</v>
       </c>
@@ -1442,12 +1456,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CACA22-017F-4E16-97D6-2BA6303A8EB1}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1623,7 +1638,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="B11" t="s">
         <v>60</v>
       </c>
@@ -1712,11 +1729,12 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A17" sqref="A17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
@@ -2034,7 +2052,7 @@
         <v>26.062000000000001</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="D19:E19" si="0">SUM(E2:E18)</f>
+        <f t="shared" ref="E19" si="0">SUM(E2:E18)</f>
         <v>22.072000000000003</v>
       </c>
     </row>

</xml_diff>